<commit_message>
Add possibility: colorful or B&W charts
</commit_message>
<xml_diff>
--- a/regions_data/Elektryczność/data.xlsx
+++ b/regions_data/Elektryczność/data.xlsx
@@ -2270,6 +2270,2081 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Liczba mieszkańców na odbiorcę</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Dolnośląskie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kujawsko-pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lubelskie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lubuskie</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Łódzkie</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Małopolskie</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mazowieckie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Opolskie</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Podkarpackie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Podlaskie</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Śląskie</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Świętokrzyskie</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Warmińsko-mazurskie</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wielkopolskie</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Zachodniopomorskie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$2:$S$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>3.3783912184922755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.27401226993865</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4304576485461435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2039843428100543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6594125383603688</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7096420581655476</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.430774326323236</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4982382022471912</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.4093527995183628</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2905615550755938</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7603348578895783</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1485918297288018</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.3912761416986772</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.623653538264489</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7459054257209239</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.6190527426160339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8EC3-4121-BC45-E4D28CAECF7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="48"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1501276944"/>
+        <c:axId val="1514278176"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Liczba odbiorców</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Dolnośląskie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kujawsko-pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lubelskie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lubuskie</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Łódzkie</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Małopolskie</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mazowieckie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Opolskie</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Podkarpackie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Podlaskie</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Śląskie</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Świętokrzyskie</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Warmińsko-mazurskie</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wielkopolskie</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Zachodniopomorskie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$N$2:$N$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>860.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>395.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>242.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>684.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>715.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1554.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>222.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>332.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>277.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>612.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1456.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>234.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>312.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>731.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>474</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8EC3-4121-BC45-E4D28CAECF7B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1358601024"/>
+        <c:axId val="1405579360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1501276944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1514278176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1514278176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Liczba mieszkańców na odbiorcę</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> energii elektrycznej</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1501276944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1405579360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Liczba odbiorców energii elektrycznej</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1358601024"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1358601024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1405579360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Moc zainstalowana na mieszkańca</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Dolnośląskie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kujawsko-pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lubelskie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lubuskie</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Łódzkie</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Małopolskie</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mazowieckie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Opolskie</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Podkarpackie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Podlaskie</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Śląskie</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Świętokrzyskie</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Warmińsko-mazurskie</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wielkopolskie</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Zachodniopomorskie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$C$2:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>#\ ##0.0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.82015996798302337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72923724109948751</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22349011475286182</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60295577703573544</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.494513077564477</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.614309261308848</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0291852430335227</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9821992730237457</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.49338080685256858</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.37452240842071349</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.76834962514286009</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5906718035449345</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4857787038385781</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.30921759292282996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0076948573380189</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8457169072961839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-54DD-44FB-90DC-BC4508EC5697}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="48"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1501276944"/>
+        <c:axId val="1514278176"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Moc zainstalowana</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Dolnośląskie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kujawsko-pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lubelskie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lubuskie</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Łódzkie</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Małopolskie</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mazowieckie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Opolskie</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Podkarpackie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Podlaskie</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Śląskie</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Świętokrzyskie</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Warmińsko-mazurskie</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wielkopolskie</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Zachodniopomorskie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$B$2:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2385.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1524.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>615.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6246.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2069.1999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5490.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1983.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1050.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>446.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1768.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7294.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1876.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>446.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3499.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3166.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-54DD-44FB-90DC-BC4508EC5697}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1358601024"/>
+        <c:axId val="1405579360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1501276944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1514278176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1514278176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Moc elektryczna zainstalowana</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> na mieszkańca [kW] </a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#\ ##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1501276944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1405579360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Moc elektryczna zaistalowana</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> [MW]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1358601024"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1358601024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1405579360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Liczba mieszkańców przypadajaca na odbiorcę (w miastach)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Dolnośląskie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kujawsko-pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lubelskie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lubuskie</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Łódzkie</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Małopolskie</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mazowieckie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Opolskie</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Podkarpackie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Podlaskie</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Śląskie</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Świętokrzyskie</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Warmińsko-mazurskie</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wielkopolskie</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Zachodniopomorskie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$2:$S$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>3.3783912184922755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.27401226993865</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4304576485461435</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2039843428100543</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6594125383603688</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7096420581655476</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.430774326323236</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4982382022471912</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.4093527995183628</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2905615550755938</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7603348578895783</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1485918297288018</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.3912761416986772</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.623653538264489</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7459054257209239</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.6190527426160339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4A01-4668-BD54-44E39BA416EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="48"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1501276944"/>
+        <c:axId val="1514278176"/>
+      </c:barChart>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Zużycie energii na mieszkańca przez sektor gospodarstw domowych [kWh]</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$A$2:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Dolnośląskie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kujawsko-pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Lubelskie</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lubuskie</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Łódzkie</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Małopolskie</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mazowieckie</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Opolskie</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Podkarpackie</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Podlaskie</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pomorskie</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Śląskie</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Świętokrzyskie</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Warmińsko-mazurskie</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Wielkopolskie</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Zachodniopomorskie</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$K$2:$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>732.34708300655643</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>698.08879651213977</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>652.77737684065062</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>674.30685078118643</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>755.55001805013785</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>793.27003006825919</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>868.87064250125275</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>779.33133371567192</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>562.65607483043993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>744.1787102804052</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>702.40917223880865</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>769.74672933960528</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>597.69976630334975</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>640.59635711896465</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>738.93207325160927</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>668.05368446763532</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4A01-4668-BD54-44E39BA416EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1358601024"/>
+        <c:axId val="1405579360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1501276944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1514278176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1514278176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Liczba mieszkańców na odbiorcę</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> energii elektrycznej</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1501276944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1405579360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Zużycie energii na mieszkańca w sektorze gospodarstw domowych </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>[kWh]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1358601024"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1358601024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1405579360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2470,6 +4545,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4483,6 +6678,1515 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5167,6 +8871,310 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1024815</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>68729</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="7" name="Grupa 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{070540E7-FF40-4E47-B475-B2833CEE552C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="14935200" y="7126941"/>
+          <a:ext cx="5758180" cy="2794000"/>
+          <a:chOff x="0" y="0"/>
+          <a:chExt cx="5758180" cy="3067050"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="8" name="Wykres 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E17F1FA7-2CFE-40A3-9488-4673D2D54429}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5758180" cy="2743200"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Pole tekstowe 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0CF6894-69CF-46B6-91DB-2C396967058A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="2800350"/>
+            <a:ext cx="5758180" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:prstClr val="white"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:spcAft>
+                <a:spcPts val="1000"/>
+              </a:spcAft>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="900" i="1">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Rysunek 5 Liczba odbiorców oraz liczba mieszkańców na 1 odbiorcę (w miastach)</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="pl-PL" sz="900" i="1">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="900" i="1">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Opracowanie własne na podstawie [5]</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>582705</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>71717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>728979</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>168156</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Wykres 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F32FE243-A271-4114-97C3-239C34251EE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>47662</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>68730</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="Grupa 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6126D5B0-C063-43EE-8797-708BB806985D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="23003435" y="4598894"/>
+          <a:ext cx="5758180" cy="3107765"/>
+          <a:chOff x="0" y="120052"/>
+          <a:chExt cx="5758180" cy="2946998"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="13" name="Wykres 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17EA21DF-7E3A-4CD7-8D44-B6B081B1EAE6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="0" y="120052"/>
+          <a:ext cx="5758180" cy="2623147"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Pole tekstowe 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E97DDD8A-2FC6-47A9-A353-333E84B2B0D3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="2800350"/>
+            <a:ext cx="5758180" cy="266700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:prstClr val="white"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+            <a:prstTxWarp prst="textNoShape">
+              <a:avLst/>
+            </a:prstTxWarp>
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:spcAft>
+                <a:spcPts val="1000"/>
+              </a:spcAft>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="900" i="1">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Rysunek 5 Liczba odbiorców oraz liczba mieszkańców na 1 odbiorcę (w miastach)</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="pl-PL" sz="900" i="1">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="900" i="1">
+                <a:solidFill>
+                  <a:srgbClr val="44546A"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Opracowanie własne na podstawie [5]</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5469,8 +9477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5537,7 +9545,7 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>2385.4</v>
       </c>
       <c r="C2" s="1">
@@ -5601,7 +9609,7 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1524.1</v>
       </c>
       <c r="C3" s="1">
@@ -5665,7 +9673,7 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>480</v>
       </c>
       <c r="C4" s="1">
@@ -5729,7 +9737,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>615.20000000000005</v>
       </c>
       <c r="C5" s="1">
@@ -5793,7 +9801,7 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>6246.6</v>
       </c>
       <c r="C6" s="1">
@@ -5857,7 +9865,7 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>2069.1999999999998</v>
       </c>
       <c r="C7" s="1">
@@ -5921,7 +9929,7 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>5490.2</v>
       </c>
       <c r="C8" s="1">
@@ -5985,7 +9993,7 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>1983.9</v>
       </c>
       <c r="C9" s="1">
@@ -6049,7 +10057,7 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>1050.5</v>
       </c>
       <c r="C10" s="1">
@@ -6113,7 +10121,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>446.4</v>
       </c>
       <c r="C11" s="1">
@@ -6177,7 +10185,7 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>1768.8</v>
       </c>
       <c r="C12" s="1">
@@ -6241,7 +10249,7 @@
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>7294.7</v>
       </c>
       <c r="C13" s="1">
@@ -6305,7 +10313,7 @@
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>1876.8</v>
       </c>
       <c r="C14" s="1">
@@ -6369,7 +10377,7 @@
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>446.5</v>
       </c>
       <c r="C15" s="1">
@@ -6433,7 +10441,7 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>3499.3</v>
       </c>
       <c r="C16" s="1">
@@ -6497,7 +10505,7 @@
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>3166.2</v>
       </c>
       <c r="C17" s="1">

</xml_diff>